<commit_message>
Sorted questions for easier access
</commit_message>
<xml_diff>
--- a/PythonPals/python_questions_extra.xlsx
+++ b/PythonPals/python_questions_extra.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Sheamus\School\Senior\Python\PythonPals\PythonPals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A415230-A0BA-4720-BDF5-0BED9571BC88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0725BD7C-98E5-4562-B217-92A2105B3988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8988" yWindow="5796" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{8E6A920C-DC8A-447C-B2E2-0D79A8F3C355}"/>
+    <workbookView xWindow="5952" yWindow="2436" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{8E6A920C-DC8A-447C-B2E2-0D79A8F3C355}"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="311">
   <si>
     <t>Number</t>
   </si>
@@ -1523,8 +1523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D33FE3-95A4-4979-84F6-48E46D9AB26E}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScale="47" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I21"/>
+    <sheetView zoomScale="47" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2156,526 +2156,589 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E03268-21A2-4836-85AC-DD011DFA9BC1}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.88671875" customWidth="1"/>
-    <col min="3" max="3" width="44.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="52.88671875" customWidth="1"/>
+    <col min="4" max="4" width="44.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>134</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>142</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>133</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>144</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>143</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>145</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>147</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>137</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>145</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>148</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>150</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>151</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>152</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>153</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>156</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>155</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>157</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>158</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>159</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>161</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>155</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>162</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>163</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>164</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>166</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>155</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>168</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>167</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>169</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>171</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>155</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>174</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>173</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>164</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>175</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>155</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" t="s">
         <v>14</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>177</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>149</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>176</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>179</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>182</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>179</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>189</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>179</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" t="s">
         <v>16</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>188</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>192</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>191</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>179</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>196</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>179</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" t="s">
+      <c r="D16" s="2"/>
+      <c r="E16" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>198</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>203</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>202</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" t="s">
+      <c r="D17" s="2"/>
+      <c r="E17" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>204</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>207</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>202</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" t="s">
+      <c r="D18" s="2"/>
+      <c r="E18" t="s">
         <v>14</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>208</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>209</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>211</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>202</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" t="s">
+      <c r="D19" s="2"/>
+      <c r="E19" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>213</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>216</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" t="s">
+      <c r="D20" s="2"/>
+      <c r="E20" t="s">
         <v>16</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>220</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>219</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>218</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>221</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>202</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" t="s">
+      <c r="D21" s="2"/>
+      <c r="E21" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>167</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>222</v>
       </c>
     </row>
@@ -2688,8 +2751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E31CADC-C786-460E-9910-31504D11CF7C}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="C5" workbookViewId="0">
+      <selection sqref="A1:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>